<commit_message>
Added Find Minumum Coins Problem
</commit_message>
<xml_diff>
--- a/Question Sheet/Question.xlsx
+++ b/Question Sheet/Question.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="469">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -730,463 +730,466 @@
     <t>Huffman Coding</t>
   </si>
   <si>
+    <t>Water Connection Problem(In Graph Solve Suing DFS)</t>
+  </si>
+  <si>
+    <t>Fractional Knapsack Problem</t>
+  </si>
+  <si>
+    <t>Greedy Algorithm to find Minimum number of Coins</t>
+  </si>
+  <si>
+    <t>Maximum trains for which stoppage can be provided</t>
+  </si>
+  <si>
+    <t>Minimum Platforms Problem</t>
+  </si>
+  <si>
+    <t>Buy Maximum Stocks if i stocks can be bought on i-th day</t>
+  </si>
+  <si>
+    <t>Find the minimum and maximum amount to buy all N candies</t>
+  </si>
+  <si>
+    <t>Minimize Cash Flow among a given set of friends who have borrowed money from each other</t>
+  </si>
+  <si>
+    <t>Minimum Cost to cut a board into squares</t>
+  </si>
+  <si>
+    <t>Check if it is possible to survive on Island</t>
+  </si>
+  <si>
+    <t>Find maximum meetings in one room</t>
+  </si>
+  <si>
+    <t>Maximum product subset of an array</t>
+  </si>
+  <si>
+    <t>Maximize array sum after K negations</t>
+  </si>
+  <si>
+    <t>Maximize the sum of arr[i]*i</t>
+  </si>
+  <si>
+    <t>Maximum sum of absolute difference of an array</t>
+  </si>
+  <si>
+    <t>Maximize sum of consecutive differences in a circular array</t>
+  </si>
+  <si>
+    <t>Minimum sum of absolute difference of pairs of two arrays</t>
+  </si>
+  <si>
+    <t>Program for Shortest Job First (or SJF) CPU Scheduling</t>
+  </si>
+  <si>
+    <t>Program for Least Recently Used (LRU) Page Replacement algorithm</t>
+  </si>
+  <si>
+    <t>Smallest subset with sum greater than all other elements</t>
+  </si>
+  <si>
+    <t>Chocolate Distribution Problem</t>
+  </si>
+  <si>
+    <t>DEFKIN -Defense of a Kingdom</t>
+  </si>
+  <si>
+    <t>DIEHARD -DIE HARD</t>
+  </si>
+  <si>
+    <t>GERGOVIA -Wine trading in Gergovia</t>
+  </si>
+  <si>
+    <t>Picking Up Chicks</t>
+  </si>
+  <si>
+    <t>CHOCOLA –Chocolate</t>
+  </si>
+  <si>
+    <t>ARRANGE -Arranging Amplifiers</t>
+  </si>
+  <si>
+    <t>K Centers Problem</t>
+  </si>
+  <si>
+    <t>Minimum Cost of ropes</t>
+  </si>
+  <si>
+    <t>Find smallest number with given number of digits and sum of digits</t>
+  </si>
+  <si>
+    <t>Find maximum sum possible equal sum of three stacks</t>
+  </si>
+  <si>
+    <t>BackTracking</t>
+  </si>
+  <si>
+    <t>Rat in a maze Problem</t>
+  </si>
+  <si>
+    <t>Printing all solutions in N-Queen Problem</t>
+  </si>
+  <si>
+    <t>Word Break Problem using Backtracking</t>
+  </si>
+  <si>
+    <t>Remove Invalid Parentheses</t>
+  </si>
+  <si>
+    <t>Sudoku Solver</t>
+  </si>
+  <si>
+    <t>m Coloring Problem</t>
+  </si>
+  <si>
+    <t>Print all palindromic partitions of a string</t>
+  </si>
+  <si>
+    <t>Subset Sum Problem</t>
+  </si>
+  <si>
+    <t>The Knight’s tour problem</t>
+  </si>
+  <si>
+    <t>Tug of War</t>
+  </si>
+  <si>
+    <t>Find shortest safe route in a path with landmines</t>
+  </si>
+  <si>
+    <t>Combinational Sum</t>
+  </si>
+  <si>
+    <t>Find Maximum number possible by doing at-most K swaps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Print all permutations of a string </t>
+  </si>
+  <si>
+    <t>Find if there is a path of more than k length from a source</t>
+  </si>
+  <si>
+    <t>Longest Possible Route in a Matrix with Hurdles</t>
+  </si>
+  <si>
+    <t>Print all possible paths from top left to bottom right of a mXn matrix</t>
+  </si>
+  <si>
+    <t>Partition of a set intoK subsets with equal sum</t>
+  </si>
+  <si>
+    <t>Find the K-th Permutation Sequence of first N natural numbers</t>
+  </si>
+  <si>
+    <t>Stacks &amp; Queues</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implement Stack from Scratch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implement Queue from Scratch</t>
+  </si>
+  <si>
+    <t>Implement 2 stack in an array</t>
+  </si>
+  <si>
+    <t>find the middle element of a stack</t>
+  </si>
+  <si>
+    <t>Implement "N" stacks in an Array</t>
+  </si>
+  <si>
+    <t>Check the expression has valid or Balanced parenthesis or not.</t>
+  </si>
+  <si>
+    <t>Reverse a String using Stack</t>
+  </si>
+  <si>
+    <t>Design a Stack that supports getMin() in O(1) time and O(1) extra space.</t>
+  </si>
+  <si>
+    <t>Find the next Greater element</t>
+  </si>
+  <si>
+    <t>The celebrity Problem</t>
+  </si>
+  <si>
+    <t>Arithmetic Expression evaluation</t>
+  </si>
+  <si>
+    <t>Evaluation of Postfix expression</t>
+  </si>
+  <si>
+    <t>Implement a method to insert an element at its bottom without using any other data structure.</t>
+  </si>
+  <si>
+    <t>Reverse a stack using recursion</t>
+  </si>
+  <si>
+    <t>Sort a Stack using recursion</t>
+  </si>
+  <si>
+    <t>Merge Overlapping Intervals</t>
+  </si>
+  <si>
+    <t>Largest rectangular Area in Histogram</t>
+  </si>
+  <si>
+    <t>Length of the Longest Valid Substring</t>
+  </si>
+  <si>
+    <t>Expression contains redundant bracket or not</t>
+  </si>
+  <si>
+    <t>Implement Stack using Queue</t>
+  </si>
+  <si>
+    <t>Implement Stack using Deque</t>
+  </si>
+  <si>
+    <t>Stack Permutations (Check if an array is stack permutation of other)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Queue using Stack  </t>
+  </si>
+  <si>
+    <t>Implement "n" queue in an array</t>
+  </si>
+  <si>
+    <t>Implement a Circular queue</t>
+  </si>
+  <si>
+    <t>LRU Cache Implementationa</t>
+  </si>
+  <si>
+    <t>Reverse a Queue using recursion</t>
+  </si>
+  <si>
+    <t>Reverse the first “K” elements of a queue</t>
+  </si>
+  <si>
+    <t>Interleave the first half of the queue with second half</t>
+  </si>
+  <si>
+    <t>Find the first circular tour that visits all Petrol Pumps</t>
+  </si>
+  <si>
+    <t>Minimum time required to rot all oranges</t>
+  </si>
+  <si>
+    <t>Distance of nearest cell having 1 in a binary matrix</t>
+  </si>
+  <si>
+    <t>First negative integer in every window of size “k”</t>
+  </si>
+  <si>
+    <t>Check if all levels of two trees are anagrams or not.</t>
+  </si>
+  <si>
+    <t>Sum of minimum and maximum elements of all subarrays of size “k”.</t>
+  </si>
+  <si>
+    <t>Minimum sum of squares of character counts in a given string after removing “k” characters.</t>
+  </si>
+  <si>
+    <t>Queue based approach or first non-repeating character in a stream.</t>
+  </si>
+  <si>
+    <t>Next Smaller Element</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>Implement a Maxheap/MinHeap using arrays and recursion.</t>
+  </si>
+  <si>
+    <t>Sort an Array using heap. (HeapSort)</t>
+  </si>
+  <si>
+    <t>Maximum of all subarrays of size k.</t>
+  </si>
+  <si>
+    <t>“k” largest element in an array</t>
+  </si>
+  <si>
+    <t>Kth smallest and largest element in an unsorted array</t>
+  </si>
+  <si>
+    <t>Merge “K” sorted arrays. [ IMP ]</t>
+  </si>
+  <si>
+    <t>Merge 2 Binary Max Heaps</t>
+  </si>
+  <si>
+    <t>Kth largest sum continuous subarrays</t>
+  </si>
+  <si>
+    <t>Leetcode- reorganize strings</t>
+  </si>
+  <si>
+    <t>Merge “K” Sorted Linked Lists [V.IMP]</t>
+  </si>
+  <si>
+    <t>Smallest range in “K” Lists</t>
+  </si>
+  <si>
+    <t>Median in a stream of Integers</t>
+  </si>
+  <si>
+    <t>Check if a Binary Tree is Heap</t>
+  </si>
+  <si>
+    <t>Connect “n” ropes with minimum cost</t>
+  </si>
+  <si>
+    <t>Convert BST to Min Heap</t>
+  </si>
+  <si>
+    <t>Convert min heap to max heap</t>
+  </si>
+  <si>
+    <t>Rearrange characters in a string such that no two adjacent are same.</t>
+  </si>
+  <si>
+    <t>Minimum sum of two numbers formed from digits of an array</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Create a Graph, print it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement BFS algorithm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement DFS Algo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detect Cycle in Directed Graph using BFS/DFS Algo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detect Cycle in UnDirected Graph using BFS/DFS Algo </t>
+  </si>
+  <si>
+    <t>Search in a Maze</t>
+  </si>
+  <si>
+    <t>Minimum Step by Knight</t>
+  </si>
+  <si>
+    <t>flood fill algo</t>
+  </si>
+  <si>
+    <t>Clone a graph</t>
+  </si>
+  <si>
+    <t>Making wired Connections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">word Ladder </t>
+  </si>
+  <si>
+    <t>Dijkstra algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Topological Sort </t>
+  </si>
+  <si>
+    <t>Minimum time taken by each job to be completed given by a Directed Acyclic Graph</t>
+  </si>
+  <si>
+    <t>Find whether it is possible to finish all tasks or not from given dependencies</t>
+  </si>
+  <si>
+    <t>Find the no. of Isalnds</t>
+  </si>
+  <si>
+    <t>Given a sorted Dictionary of an Alien Language, find order of characters</t>
+  </si>
+  <si>
+    <t>Implement Kruksal’sAlgorithm</t>
+  </si>
+  <si>
+    <t>Implement Prim’s Algorithm</t>
+  </si>
+  <si>
+    <t>Total no. of Spanning tree in a graph</t>
+  </si>
+  <si>
+    <t>Implement Bellman Ford Algorithm</t>
+  </si>
+  <si>
+    <t>Implement Floyd warshallAlgorithm</t>
+  </si>
+  <si>
+    <t>Travelling Salesman Problem</t>
+  </si>
+  <si>
+    <t>Graph ColouringProblem</t>
+  </si>
+  <si>
+    <t>Snake and Ladders Problem</t>
+  </si>
+  <si>
+    <t>Find bridge in a graph</t>
+  </si>
+  <si>
+    <t>Count Strongly connected Components(Kosaraju Algo)</t>
+  </si>
+  <si>
+    <t>Check whether a graph is Bipartite or Not</t>
+  </si>
+  <si>
+    <t>Detect Negative cycle in a graph</t>
+  </si>
+  <si>
+    <t>Longest path in a Directed Acyclic Graph</t>
+  </si>
+  <si>
+    <t>Journey to the Moon</t>
+  </si>
+  <si>
+    <t>Cheapest Flights Within K Stops</t>
+  </si>
+  <si>
+    <t>Oliver and the Game</t>
+  </si>
+  <si>
+    <t>Water Jug problem using BFS</t>
+  </si>
+  <si>
+    <t>Find if there is a path of more thank length from a source</t>
+  </si>
+  <si>
+    <t>M-ColouringProblem</t>
+  </si>
+  <si>
+    <t>Minimum edges to reverse o make path from source to destination</t>
+  </si>
+  <si>
+    <t>Paths to travel each nodes using each edge(Seven Bridges)</t>
+  </si>
+  <si>
+    <t>Vertex Cover Problem</t>
+  </si>
+  <si>
+    <t>Chinese Postman or Route Inspection</t>
+  </si>
+  <si>
+    <t>Number of Triangles in a Directed and Undirected Graph</t>
+  </si>
+  <si>
+    <t>Minimise the cashflow among a given set of friends who have borrowed money from each other</t>
+  </si>
+  <si>
+    <t>Two Clique Problem</t>
+  </si>
+  <si>
     <t>Water Connection Problem</t>
-  </si>
-  <si>
-    <t>Fractional Knapsack Problem</t>
-  </si>
-  <si>
-    <t>Greedy Algorithm to find Minimum number of Coins</t>
-  </si>
-  <si>
-    <t>Maximum trains for which stoppage can be provided</t>
-  </si>
-  <si>
-    <t>Minimum Platforms Problem</t>
-  </si>
-  <si>
-    <t>Buy Maximum Stocks if i stocks can be bought on i-th day</t>
-  </si>
-  <si>
-    <t>Find the minimum and maximum amount to buy all N candies</t>
-  </si>
-  <si>
-    <t>Minimize Cash Flow among a given set of friends who have borrowed money from each other</t>
-  </si>
-  <si>
-    <t>Minimum Cost to cut a board into squares</t>
-  </si>
-  <si>
-    <t>Check if it is possible to survive on Island</t>
-  </si>
-  <si>
-    <t>Find maximum meetings in one room</t>
-  </si>
-  <si>
-    <t>Maximum product subset of an array</t>
-  </si>
-  <si>
-    <t>Maximize array sum after K negations</t>
-  </si>
-  <si>
-    <t>Maximize the sum of arr[i]*i</t>
-  </si>
-  <si>
-    <t>Maximum sum of absolute difference of an array</t>
-  </si>
-  <si>
-    <t>Maximize sum of consecutive differences in a circular array</t>
-  </si>
-  <si>
-    <t>Minimum sum of absolute difference of pairs of two arrays</t>
-  </si>
-  <si>
-    <t>Program for Shortest Job First (or SJF) CPU Scheduling</t>
-  </si>
-  <si>
-    <t>Program for Least Recently Used (LRU) Page Replacement algorithm</t>
-  </si>
-  <si>
-    <t>Smallest subset with sum greater than all other elements</t>
-  </si>
-  <si>
-    <t>Chocolate Distribution Problem</t>
-  </si>
-  <si>
-    <t>DEFKIN -Defense of a Kingdom</t>
-  </si>
-  <si>
-    <t>DIEHARD -DIE HARD</t>
-  </si>
-  <si>
-    <t>GERGOVIA -Wine trading in Gergovia</t>
-  </si>
-  <si>
-    <t>Picking Up Chicks</t>
-  </si>
-  <si>
-    <t>CHOCOLA –Chocolate</t>
-  </si>
-  <si>
-    <t>ARRANGE -Arranging Amplifiers</t>
-  </si>
-  <si>
-    <t>K Centers Problem</t>
-  </si>
-  <si>
-    <t>Minimum Cost of ropes</t>
-  </si>
-  <si>
-    <t>Find smallest number with given number of digits and sum of digits</t>
-  </si>
-  <si>
-    <t>Find maximum sum possible equal sum of three stacks</t>
-  </si>
-  <si>
-    <t>BackTracking</t>
-  </si>
-  <si>
-    <t>Rat in a maze Problem</t>
-  </si>
-  <si>
-    <t>Printing all solutions in N-Queen Problem</t>
-  </si>
-  <si>
-    <t>Word Break Problem using Backtracking</t>
-  </si>
-  <si>
-    <t>Remove Invalid Parentheses</t>
-  </si>
-  <si>
-    <t>Sudoku Solver</t>
-  </si>
-  <si>
-    <t>m Coloring Problem</t>
-  </si>
-  <si>
-    <t>Print all palindromic partitions of a string</t>
-  </si>
-  <si>
-    <t>Subset Sum Problem</t>
-  </si>
-  <si>
-    <t>The Knight’s tour problem</t>
-  </si>
-  <si>
-    <t>Tug of War</t>
-  </si>
-  <si>
-    <t>Find shortest safe route in a path with landmines</t>
-  </si>
-  <si>
-    <t>Combinational Sum</t>
-  </si>
-  <si>
-    <t>Find Maximum number possible by doing at-most K swaps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print all permutations of a string </t>
-  </si>
-  <si>
-    <t>Find if there is a path of more than k length from a source</t>
-  </si>
-  <si>
-    <t>Longest Possible Route in a Matrix with Hurdles</t>
-  </si>
-  <si>
-    <t>Print all possible paths from top left to bottom right of a mXn matrix</t>
-  </si>
-  <si>
-    <t>Partition of a set intoK subsets with equal sum</t>
-  </si>
-  <si>
-    <t>Find the K-th Permutation Sequence of first N natural numbers</t>
-  </si>
-  <si>
-    <t>Stacks &amp; Queues</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implement Stack from Scratch</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implement Queue from Scratch</t>
-  </si>
-  <si>
-    <t>Implement 2 stack in an array</t>
-  </si>
-  <si>
-    <t>find the middle element of a stack</t>
-  </si>
-  <si>
-    <t>Implement "N" stacks in an Array</t>
-  </si>
-  <si>
-    <t>Check the expression has valid or Balanced parenthesis or not.</t>
-  </si>
-  <si>
-    <t>Reverse a String using Stack</t>
-  </si>
-  <si>
-    <t>Design a Stack that supports getMin() in O(1) time and O(1) extra space.</t>
-  </si>
-  <si>
-    <t>Find the next Greater element</t>
-  </si>
-  <si>
-    <t>The celebrity Problem</t>
-  </si>
-  <si>
-    <t>Arithmetic Expression evaluation</t>
-  </si>
-  <si>
-    <t>Evaluation of Postfix expression</t>
-  </si>
-  <si>
-    <t>Implement a method to insert an element at its bottom without using any other data structure.</t>
-  </si>
-  <si>
-    <t>Reverse a stack using recursion</t>
-  </si>
-  <si>
-    <t>Sort a Stack using recursion</t>
-  </si>
-  <si>
-    <t>Merge Overlapping Intervals</t>
-  </si>
-  <si>
-    <t>Largest rectangular Area in Histogram</t>
-  </si>
-  <si>
-    <t>Length of the Longest Valid Substring</t>
-  </si>
-  <si>
-    <t>Expression contains redundant bracket or not</t>
-  </si>
-  <si>
-    <t>Implement Stack using Queue</t>
-  </si>
-  <si>
-    <t>Implement Stack using Deque</t>
-  </si>
-  <si>
-    <t>Stack Permutations (Check if an array is stack permutation of other)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement Queue using Stack  </t>
-  </si>
-  <si>
-    <t>Implement "n" queue in an array</t>
-  </si>
-  <si>
-    <t>Implement a Circular queue</t>
-  </si>
-  <si>
-    <t>LRU Cache Implementationa</t>
-  </si>
-  <si>
-    <t>Reverse a Queue using recursion</t>
-  </si>
-  <si>
-    <t>Reverse the first “K” elements of a queue</t>
-  </si>
-  <si>
-    <t>Interleave the first half of the queue with second half</t>
-  </si>
-  <si>
-    <t>Find the first circular tour that visits all Petrol Pumps</t>
-  </si>
-  <si>
-    <t>Minimum time required to rot all oranges</t>
-  </si>
-  <si>
-    <t>Distance of nearest cell having 1 in a binary matrix</t>
-  </si>
-  <si>
-    <t>First negative integer in every window of size “k”</t>
-  </si>
-  <si>
-    <t>Check if all levels of two trees are anagrams or not.</t>
-  </si>
-  <si>
-    <t>Sum of minimum and maximum elements of all subarrays of size “k”.</t>
-  </si>
-  <si>
-    <t>Minimum sum of squares of character counts in a given string after removing “k” characters.</t>
-  </si>
-  <si>
-    <t>Queue based approach or first non-repeating character in a stream.</t>
-  </si>
-  <si>
-    <t>Next Smaller Element</t>
-  </si>
-  <si>
-    <t>Heap</t>
-  </si>
-  <si>
-    <t>Implement a Maxheap/MinHeap using arrays and recursion.</t>
-  </si>
-  <si>
-    <t>Sort an Array using heap. (HeapSort)</t>
-  </si>
-  <si>
-    <t>Maximum of all subarrays of size k.</t>
-  </si>
-  <si>
-    <t>“k” largest element in an array</t>
-  </si>
-  <si>
-    <t>Kth smallest and largest element in an unsorted array</t>
-  </si>
-  <si>
-    <t>Merge “K” sorted arrays. [ IMP ]</t>
-  </si>
-  <si>
-    <t>Merge 2 Binary Max Heaps</t>
-  </si>
-  <si>
-    <t>Kth largest sum continuous subarrays</t>
-  </si>
-  <si>
-    <t>Leetcode- reorganize strings</t>
-  </si>
-  <si>
-    <t>Merge “K” Sorted Linked Lists [V.IMP]</t>
-  </si>
-  <si>
-    <t>Smallest range in “K” Lists</t>
-  </si>
-  <si>
-    <t>Median in a stream of Integers</t>
-  </si>
-  <si>
-    <t>Check if a Binary Tree is Heap</t>
-  </si>
-  <si>
-    <t>Connect “n” ropes with minimum cost</t>
-  </si>
-  <si>
-    <t>Convert BST to Min Heap</t>
-  </si>
-  <si>
-    <t>Convert min heap to max heap</t>
-  </si>
-  <si>
-    <t>Rearrange characters in a string such that no two adjacent are same.</t>
-  </si>
-  <si>
-    <t>Minimum sum of two numbers formed from digits of an array</t>
-  </si>
-  <si>
-    <t>Graph</t>
-  </si>
-  <si>
-    <t>Create a Graph, print it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement BFS algorithm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement DFS Algo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detect Cycle in Directed Graph using BFS/DFS Algo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detect Cycle in UnDirected Graph using BFS/DFS Algo </t>
-  </si>
-  <si>
-    <t>Search in a Maze</t>
-  </si>
-  <si>
-    <t>Minimum Step by Knight</t>
-  </si>
-  <si>
-    <t>flood fill algo</t>
-  </si>
-  <si>
-    <t>Clone a graph</t>
-  </si>
-  <si>
-    <t>Making wired Connections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">word Ladder </t>
-  </si>
-  <si>
-    <t>Dijkstra algo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement Topological Sort </t>
-  </si>
-  <si>
-    <t>Minimum time taken by each job to be completed given by a Directed Acyclic Graph</t>
-  </si>
-  <si>
-    <t>Find whether it is possible to finish all tasks or not from given dependencies</t>
-  </si>
-  <si>
-    <t>Find the no. of Isalnds</t>
-  </si>
-  <si>
-    <t>Given a sorted Dictionary of an Alien Language, find order of characters</t>
-  </si>
-  <si>
-    <t>Implement Kruksal’sAlgorithm</t>
-  </si>
-  <si>
-    <t>Implement Prim’s Algorithm</t>
-  </si>
-  <si>
-    <t>Total no. of Spanning tree in a graph</t>
-  </si>
-  <si>
-    <t>Implement Bellman Ford Algorithm</t>
-  </si>
-  <si>
-    <t>Implement Floyd warshallAlgorithm</t>
-  </si>
-  <si>
-    <t>Travelling Salesman Problem</t>
-  </si>
-  <si>
-    <t>Graph ColouringProblem</t>
-  </si>
-  <si>
-    <t>Snake and Ladders Problem</t>
-  </si>
-  <si>
-    <t>Find bridge in a graph</t>
-  </si>
-  <si>
-    <t>Count Strongly connected Components(Kosaraju Algo)</t>
-  </si>
-  <si>
-    <t>Check whether a graph is Bipartite or Not</t>
-  </si>
-  <si>
-    <t>Detect Negative cycle in a graph</t>
-  </si>
-  <si>
-    <t>Longest path in a Directed Acyclic Graph</t>
-  </si>
-  <si>
-    <t>Journey to the Moon</t>
-  </si>
-  <si>
-    <t>Cheapest Flights Within K Stops</t>
-  </si>
-  <si>
-    <t>Oliver and the Game</t>
-  </si>
-  <si>
-    <t>Water Jug problem using BFS</t>
-  </si>
-  <si>
-    <t>Find if there is a path of more thank length from a source</t>
-  </si>
-  <si>
-    <t>M-ColouringProblem</t>
-  </si>
-  <si>
-    <t>Minimum edges to reverse o make path from source to destination</t>
-  </si>
-  <si>
-    <t>Paths to travel each nodes using each edge(Seven Bridges)</t>
-  </si>
-  <si>
-    <t>Vertex Cover Problem</t>
-  </si>
-  <si>
-    <t>Chinese Postman or Route Inspection</t>
-  </si>
-  <si>
-    <t>Number of Triangles in a Directed and Undirected Graph</t>
-  </si>
-  <si>
-    <t>Minimise the cashflow among a given set of friends who have borrowed money from each other</t>
-  </si>
-  <si>
-    <t>Two Clique Problem</t>
   </si>
   <si>
     <t>Trie</t>
@@ -6488,8 +6491,12 @@
       <c r="D399" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="400" customHeight="1" ht="19.5">
-      <c r="A400" s="1"/>
-      <c r="B400" s="1"/>
+      <c r="A400" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>391</v>
+      </c>
       <c r="C400" s="1"/>
       <c r="D400" s="2"/>
     </row>
@@ -6501,10 +6508,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="402" customHeight="1" ht="19.5">
       <c r="A402" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>8</v>
@@ -6513,10 +6520,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="403" customHeight="1" ht="19.5">
       <c r="A403" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>8</v>
@@ -6525,10 +6532,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="404" customHeight="1" ht="19.5">
       <c r="A404" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>8</v>
@@ -6537,7 +6544,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="405" customHeight="1" ht="19.5">
       <c r="A405" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B405" s="1" t="s">
         <v>93</v>
@@ -6549,10 +6556,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="406" customHeight="1" ht="19.5">
       <c r="A406" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C406" s="1" t="s">
         <v>8</v>
@@ -6561,10 +6568,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="407" customHeight="1" ht="19.5">
       <c r="A407" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C407" s="1" t="s">
         <v>8</v>
@@ -6585,10 +6592,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="410" customHeight="1" ht="19.5">
       <c r="A410" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C410" s="1" t="s">
         <v>8</v>
@@ -6597,10 +6604,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="411" customHeight="1" ht="19.5">
       <c r="A411" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C411" s="1" t="s">
         <v>8</v>
@@ -6609,10 +6616,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="412" customHeight="1" ht="19.5">
       <c r="A412" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C412" s="1" t="s">
         <v>8</v>
@@ -6621,10 +6628,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="413" customHeight="1" ht="19.5">
       <c r="A413" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C413" s="1" t="s">
         <v>8</v>
@@ -6633,10 +6640,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="414" customHeight="1" ht="19.5">
       <c r="A414" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C414" s="1" t="s">
         <v>8</v>
@@ -6645,10 +6652,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="415" customHeight="1" ht="19.5">
       <c r="A415" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C415" s="1" t="s">
         <v>8</v>
@@ -6657,10 +6664,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="416" customHeight="1" ht="19.5">
       <c r="A416" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C416" s="1" t="s">
         <v>8</v>
@@ -6669,7 +6676,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="417" customHeight="1" ht="19.5">
       <c r="A417" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B417" s="1" t="s">
         <v>277</v>
@@ -6681,10 +6688,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="418" customHeight="1" ht="19.5">
       <c r="A418" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C418" s="1" t="s">
         <v>8</v>
@@ -6693,10 +6700,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="419" customHeight="1" ht="19.5">
       <c r="A419" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C419" s="1" t="s">
         <v>8</v>
@@ -6705,10 +6712,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="420" customHeight="1" ht="19.5">
       <c r="A420" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C420" s="1" t="s">
         <v>8</v>
@@ -6717,10 +6724,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="421" customHeight="1" ht="19.5">
       <c r="A421" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C421" s="1" t="s">
         <v>8</v>
@@ -6729,10 +6736,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="422" customHeight="1" ht="19.5">
       <c r="A422" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>8</v>
@@ -6741,10 +6748,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="423" customHeight="1" ht="19.5">
       <c r="A423" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>8</v>
@@ -6753,10 +6760,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="424" customHeight="1" ht="19.5">
       <c r="A424" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C424" s="1" t="s">
         <v>8</v>
@@ -6765,10 +6772,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="425" customHeight="1" ht="19.5">
       <c r="A425" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>8</v>
@@ -6777,10 +6784,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="426" customHeight="1" ht="19.5">
       <c r="A426" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C426" s="1" t="s">
         <v>8</v>
@@ -6789,10 +6796,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="427" customHeight="1" ht="19.5">
       <c r="A427" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C427" s="1" t="s">
         <v>8</v>
@@ -6801,10 +6808,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="428" customHeight="1" ht="19.5">
       <c r="A428" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C428" s="1" t="s">
         <v>8</v>
@@ -6813,10 +6820,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="429" customHeight="1" ht="19.5">
       <c r="A429" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C429" s="1" t="s">
         <v>8</v>
@@ -6825,10 +6832,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="430" customHeight="1" ht="19.5">
       <c r="A430" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C430" s="1" t="s">
         <v>8</v>
@@ -6837,10 +6844,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="431" customHeight="1" ht="19.5">
       <c r="A431" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C431" s="1" t="s">
         <v>8</v>
@@ -6849,10 +6856,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="432" customHeight="1" ht="19.5">
       <c r="A432" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C432" s="1" t="s">
         <v>8</v>
@@ -6861,10 +6868,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="433" customHeight="1" ht="19.5">
       <c r="A433" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C433" s="1" t="s">
         <v>8</v>
@@ -6873,10 +6880,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="434" customHeight="1" ht="19.5">
       <c r="A434" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C434" s="1" t="s">
         <v>8</v>
@@ -6885,10 +6892,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="435" customHeight="1" ht="19.5">
       <c r="A435" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C435" s="1" t="s">
         <v>8</v>
@@ -6897,10 +6904,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="436" customHeight="1" ht="19.5">
       <c r="A436" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C436" s="1" t="s">
         <v>8</v>
@@ -6909,10 +6916,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="437" customHeight="1" ht="19.5">
       <c r="A437" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C437" s="1" t="s">
         <v>8</v>
@@ -6921,10 +6928,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="438" customHeight="1" ht="19.5">
       <c r="A438" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C438" s="1" t="s">
         <v>8</v>
@@ -6933,10 +6940,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="439" customHeight="1" ht="19.5">
       <c r="A439" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C439" s="1" t="s">
         <v>8</v>
@@ -6945,10 +6952,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="440" customHeight="1" ht="19.5">
       <c r="A440" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C440" s="1" t="s">
         <v>8</v>
@@ -6957,10 +6964,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="441" customHeight="1" ht="19.5">
       <c r="A441" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C441" s="1" t="s">
         <v>8</v>
@@ -6969,10 +6976,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="442" customHeight="1" ht="19.5">
       <c r="A442" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C442" s="1" t="s">
         <v>8</v>
@@ -6981,10 +6988,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="443" customHeight="1" ht="19.5">
       <c r="A443" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C443" s="1" t="s">
         <v>8</v>
@@ -6993,10 +7000,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="444" customHeight="1" ht="19.5">
       <c r="A444" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C444" s="1" t="s">
         <v>8</v>
@@ -7005,10 +7012,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="445" customHeight="1" ht="19.5">
       <c r="A445" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C445" s="1" t="s">
         <v>8</v>
@@ -7017,10 +7024,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="446" customHeight="1" ht="19.5">
       <c r="A446" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C446" s="1" t="s">
         <v>8</v>
@@ -7029,10 +7036,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="447" customHeight="1" ht="19.5">
       <c r="A447" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C447" s="1" t="s">
         <v>8</v>
@@ -7041,10 +7048,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="448" customHeight="1" ht="19.5">
       <c r="A448" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C448" s="1" t="s">
         <v>8</v>
@@ -7053,10 +7060,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="449" customHeight="1" ht="19.5">
       <c r="A449" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C449" s="1" t="s">
         <v>8</v>
@@ -7065,10 +7072,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="450" customHeight="1" ht="19.5">
       <c r="A450" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C450" s="1" t="s">
         <v>8</v>
@@ -7077,10 +7084,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="451" customHeight="1" ht="19.5">
       <c r="A451" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C451" s="1" t="s">
         <v>8</v>
@@ -7089,10 +7096,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="452" customHeight="1" ht="19.5">
       <c r="A452" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C452" s="1" t="s">
         <v>8</v>
@@ -7101,10 +7108,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="453" customHeight="1" ht="19.5">
       <c r="A453" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C453" s="1" t="s">
         <v>8</v>
@@ -7113,10 +7120,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="454" customHeight="1" ht="19.5">
       <c r="A454" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C454" s="1" t="s">
         <v>8</v>
@@ -7125,10 +7132,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="455" customHeight="1" ht="19.5">
       <c r="A455" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C455" s="1" t="s">
         <v>8</v>
@@ -7137,10 +7144,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="456" customHeight="1" ht="19.5">
       <c r="A456" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C456" s="1" t="s">
         <v>8</v>
@@ -7149,10 +7156,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="457" customHeight="1" ht="19.5">
       <c r="A457" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C457" s="1" t="s">
         <v>8</v>
@@ -7161,10 +7168,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="458" customHeight="1" ht="19.5">
       <c r="A458" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C458" s="1" t="s">
         <v>8</v>
@@ -7173,10 +7180,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="459" customHeight="1" ht="19.5">
       <c r="A459" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C459" s="1" t="s">
         <v>8</v>
@@ -7185,10 +7192,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="460" customHeight="1" ht="19.5">
       <c r="A460" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C460" s="1" t="s">
         <v>8</v>
@@ -7197,10 +7204,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="461" customHeight="1" ht="19.5">
       <c r="A461" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C461" s="1" t="s">
         <v>8</v>
@@ -7209,10 +7216,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="462" customHeight="1" ht="19.5">
       <c r="A462" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C462" s="1" t="s">
         <v>8</v>
@@ -7221,10 +7228,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="463" customHeight="1" ht="19.5">
       <c r="A463" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C463" s="1" t="s">
         <v>8</v>
@@ -7233,10 +7240,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="464" customHeight="1" ht="19.5">
       <c r="A464" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C464" s="1" t="s">
         <v>8</v>
@@ -7245,10 +7252,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="465" customHeight="1" ht="19.5">
       <c r="A465" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C465" s="1" t="s">
         <v>8</v>
@@ -7257,10 +7264,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="466" customHeight="1" ht="19.5">
       <c r="A466" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C466" s="1" t="s">
         <v>8</v>
@@ -7269,10 +7276,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="467" customHeight="1" ht="19.5">
       <c r="A467" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C467" s="1" t="s">
         <v>8</v>
@@ -7281,10 +7288,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="468" customHeight="1" ht="19.5">
       <c r="A468" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C468" s="1" t="s">
         <v>8</v>
@@ -7293,10 +7300,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="469" customHeight="1" ht="19.5">
       <c r="A469" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C469" s="1" t="s">
         <v>8</v>
@@ -7317,10 +7324,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="472" customHeight="1" ht="19.5">
       <c r="A472" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C472" s="1" t="s">
         <v>8</v>
@@ -7329,10 +7336,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="473" customHeight="1" ht="19.5">
       <c r="A473" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C473" s="1" t="s">
         <v>8</v>
@@ -7341,10 +7348,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="474" customHeight="1" ht="19.5">
       <c r="A474" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C474" s="1" t="s">
         <v>8</v>
@@ -7353,10 +7360,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="475" customHeight="1" ht="19.5">
       <c r="A475" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C475" s="1" t="s">
         <v>8</v>
@@ -7365,10 +7372,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="476" customHeight="1" ht="19.5">
       <c r="A476" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C476" s="1" t="s">
         <v>8</v>
@@ -7377,10 +7384,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="477" customHeight="1" ht="19.5">
       <c r="A477" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C477" s="1" t="s">
         <v>8</v>
@@ -7389,10 +7396,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="478" customHeight="1" ht="19.5">
       <c r="A478" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C478" s="1" t="s">
         <v>8</v>
@@ -7401,10 +7408,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="479" customHeight="1" ht="19.5">
       <c r="A479" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C479" s="1" t="s">
         <v>8</v>
@@ -7413,10 +7420,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="480" customHeight="1" ht="19.5">
       <c r="A480" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C480" s="1" t="s">
         <v>8</v>
@@ -7425,10 +7432,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="481" customHeight="1" ht="19.5">
       <c r="A481" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C481" s="1" t="s">
         <v>8</v>

</xml_diff>